<commit_message>
Increased the Exist timeout for synchronization of intially bringing up the Shared Space customization.  Base 20 seconds wasn't enough.
</commit_message>
<xml_diff>
--- a/uft-one-ai-ppm-octane-integration-setup/Default.xlsx
+++ b/uft-one-ai-ppm-octane-integration-setup/Default.xlsx
@@ -541,7 +541,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -603,15 +603,6 @@
       <c s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="1"/>
-      <c s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>